<commit_message>
fixed up careers page look on phone
</commit_message>
<xml_diff>
--- a/src/data/opportunities_template.xlsx
+++ b/src/data/opportunities_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PengOlivia/Desktop/Uni/SUDATA/2026 tech/SUDATA-Website/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872079BE-0B8C-AB47-AB20-9A58C4926468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0E3318-0056-5C4A-BF60-1610D151C6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -122,9 +122,6 @@
     <t>/sponsors/current-sponsors/jane-street.png</t>
   </si>
   <si>
-    <t>Apply to Jane Street's full range of roles — internships, new grad positions, and experienced hires — through their dedicated Australian application portal. Rolling applications, apply any time.</t>
-  </si>
-  <si>
     <t>https://www.janestreet.com/apply-portal-aus/</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   </si>
   <si>
     <t>IMC Trading is offering internship positions for students interested in quantitative trading, software engineering, and market making. Join a global team of problem solvers using technology and algorithms to trade in financial markets worldwide.</t>
+  </si>
+  <si>
+    <t>Portal is a multi-day immersive experience designed to give students a real insight into how Jane Street approaches trading, research, and technology. Selected participants will take part in strategic games, hands-on technical sessions, and talks led by industry professionals.</t>
   </si>
 </sst>
 </file>
@@ -653,9 +653,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -714,7 +714,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" s="6">
         <v>46089</v>
@@ -723,15 +723,15 @@
         <v>23</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>31</v>
@@ -743,19 +743,19 @@
         <v>1</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -772,7 +772,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>20</v>
@@ -781,7 +781,7 @@
         <v>23</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>29</v>

</xml_diff>